<commit_message>
updates to coral evenness function
</commit_message>
<xml_diff>
--- a/ecosystemservices/ReefConditionCriteria.xlsx
+++ b/ecosystemservices/ReefConditionCriteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KenAnthony\Documents\GitHub\ADRIA_repo\ecosystemservices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E70CF9-175B-4F4C-995C-28E02D49D96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36B89E0-AF2A-4031-8591-2F054CCBEB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{36D98FBD-8F30-492B-9B88-2E3C82D25DD6}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -472,7 +472,7 @@
         <v>0.3</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
         <v>0.2</v>
@@ -501,7 +501,7 @@
         <v>0.25</v>
       </c>
       <c r="C3">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="D3">
         <v>0.15</v>
@@ -530,7 +530,7 @@
         <v>0.2</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="D4">
         <v>0.1</v>
@@ -559,7 +559,7 @@
         <v>0.1</v>
       </c>
       <c r="C5">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="D5">
         <v>0.05</v>
@@ -588,7 +588,7 @@
         <v>0.05</v>
       </c>
       <c r="C6">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D6">
         <v>0</v>

</xml_diff>